<commit_message>
wrote firstdayinit and closingscripts, closePosition, switch to livequotes
</commit_message>
<xml_diff>
--- a/src/backtester/significant_dates.xlsx
+++ b/src/backtester/significant_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxyan\OneDrive\Documents\Programming\Trading\AAPL2023 Options\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxyan\OneDrive\Documents\Github\Options-Backtesting-Python\src\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{095721E2-2416-45E4-BAD1-C182CE7368B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FB0884-377B-4B43-8DE0-AF30CB3CE8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52335" yWindow="3330" windowWidth="20010" windowHeight="15975" xr2:uid="{5B127225-11A8-4F36-9497-2D28A15E7E76}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5B127225-11A8-4F36-9497-2D28A15E7E76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,67 +36,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Vol</t>
-  </si>
-  <si>
-    <t>Dir</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>CPI report</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Link to CPI report page</t>
   </si>
   <si>
-    <t>link to labor report calendar</t>
-  </si>
-  <si>
-    <t>link to fed calendar</t>
-  </si>
-  <si>
     <t>NVDA 5000 series launch</t>
   </si>
   <si>
     <t>Fed meeting</t>
   </si>
   <si>
-    <t>Time before</t>
-  </si>
-  <si>
-    <t>Labor report. expecting negative news</t>
-  </si>
-  <si>
     <t>HOW TO USE</t>
   </si>
   <si>
-    <t xml:space="preserve">Place date of event in date column. Leave vol and dir blank for defaultL: slight vol increase. </t>
-  </si>
-  <si>
     <t>If more vol expected than usual, put a vol number &gt;.5</t>
   </si>
   <si>
     <t>if positive dir expected, put a dir number &gt;.5</t>
   </si>
   <si>
-    <t>use the links below to add more dates to calendar. Enter newest dates first</t>
+    <t>time_impact</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>vol</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place date of event in date column. Leave vol and dir blank for default (slight vol increase) </t>
+  </si>
+  <si>
+    <t>Input a "-1" into vol to signify market closed day</t>
+  </si>
+  <si>
+    <t>Use the links below to add more dates to calendar. Enter newest dates first</t>
+  </si>
+  <si>
+    <t>Link to fed calendar</t>
+  </si>
+  <si>
+    <t>Link to labor report calendar</t>
+  </si>
+  <si>
+    <t>October CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>November CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>December CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>January CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>Febuary CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>March CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>April CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>May CPI Report (8:30am)</t>
+  </si>
+  <si>
+    <t>October Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>expecting negative news</t>
+  </si>
+  <si>
+    <t>November Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>December Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>January Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>Febuary Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>Marhc Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>April Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>May Labor Report (8:30am)</t>
+  </si>
+  <si>
+    <t>Leave time_impact column blank for now</t>
+  </si>
+  <si>
+    <t>Fed Meeting  (18-19th)</t>
+  </si>
+  <si>
+    <t>Fed Meeting (28-29th)</t>
+  </si>
+  <si>
+    <t>Fed Meeting ( 6-7th)</t>
+  </si>
+  <si>
+    <t>new years</t>
+  </si>
+  <si>
+    <t>market closed</t>
+  </si>
+  <si>
+    <t>martin luther</t>
+  </si>
+  <si>
+    <t>good Friday</t>
+  </si>
+  <si>
+    <t>washingtons bday</t>
+  </si>
+  <si>
+    <t>higher volatility</t>
+  </si>
+  <si>
+    <t>vol and dir inputs here are supplemented into calculation, not overriding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,14 +214,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,42 +557,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78BBBB2-F02D-4EC0-B902-2A155DB8A109}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45664</v>
+        <v>45819</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -502,61 +607,273 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45643</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>45815</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45637</v>
+        <v>45814</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>45790</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45779</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45765</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45757</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45751</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45735</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45728</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45723</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45705</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45700</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45695</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45686</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45677</v>
+      </c>
+      <c r="B17">
+        <v>-1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45672</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45671</v>
+      </c>
+      <c r="B19">
+        <v>0.3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45667</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45664</v>
+      </c>
+      <c r="B21">
+        <v>0.6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45643</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45637</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>45632</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" t="s">
-        <v>7</v>
+      <c r="C25">
+        <v>0.3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45609</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45597</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{8CEF2B51-A71D-48B7-8390-DE09F57B1101}"/>
+    <hyperlink ref="G11" r:id="rId2" xr:uid="{E130A780-EA49-44A1-AF36-3BE1E41309DA}"/>
+    <hyperlink ref="G12" r:id="rId3" xr:uid="{1F3C2790-2FA8-432D-BCBA-FA363C1DEC5F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated sig_dates holidays, working on BT
</commit_message>
<xml_diff>
--- a/src/backtester/significant_dates.xlsx
+++ b/src/backtester/significant_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxyan\OneDrive\Documents\Github\Options-Backtesting-Python\src\core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxyan\OneDrive\Documents\Github\Options-Backtesting-Python\src\live\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FB0884-377B-4B43-8DE0-AF30CB3CE8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A59EBA8-1216-44E4-AEBD-68013B77DC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5B127225-11A8-4F36-9497-2D28A15E7E76}"/>
+    <workbookView xWindow="1125" yWindow="0" windowWidth="20010" windowHeight="15480" xr2:uid="{5B127225-11A8-4F36-9497-2D28A15E7E76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Link to CPI report page</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>vol and dir inputs here are supplemented into calculation, not overriding</t>
+  </si>
+  <si>
+    <t>Link to NYSE calendar</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,6 +656,9 @@
       <c r="A7" s="1">
         <v>45765</v>
       </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
       <c r="E7" t="s">
         <v>42</v>
       </c>
@@ -719,11 +725,17 @@
       <c r="A13" s="1">
         <v>45705</v>
       </c>
+      <c r="B13">
+        <v>-1</v>
+      </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
       <c r="F13" t="s">
         <v>40</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,6 +885,7 @@
     <hyperlink ref="G10" r:id="rId1" xr:uid="{8CEF2B51-A71D-48B7-8390-DE09F57B1101}"/>
     <hyperlink ref="G11" r:id="rId2" xr:uid="{E130A780-EA49-44A1-AF36-3BE1E41309DA}"/>
     <hyperlink ref="G12" r:id="rId3" xr:uid="{1F3C2790-2FA8-432D-BCBA-FA363C1DEC5F}"/>
+    <hyperlink ref="G13" r:id="rId4" xr:uid="{CA96B458-6A6D-488B-BFDC-DEB30B33CBF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>